<commit_message>
Separación manual (problema .append())
</commit_message>
<xml_diff>
--- a/data/reemplazos_manual/reemplazos_manual.xlsx
+++ b/data/reemplazos_manual/reemplazos_manual.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aricop/Desktop/ISA/Recomendador/recomendador_v2/data/reemplazos_manual/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A163C55-298B-574E-958F-BDDE5D4547C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C12AE7-DB37-304A-B7AB-DC6BDB9C9E62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" activeTab="7" xr2:uid="{0F8FBB99-2BFB-F445-9E1D-14AC441B556A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25740" windowHeight="21940" xr2:uid="{0F8FBB99-2BFB-F445-9E1D-14AC441B556A}"/>
   </bookViews>
   <sheets>
     <sheet name="T-PAP(C)_T-ACE" sheetId="1" r:id="rId1"/>
@@ -2299,9 +2299,6 @@
     <t>Reemplazos</t>
   </si>
   <si>
-    <t>muestra de aceit</t>
-  </si>
-  <si>
     <t>realizar muestreo analisis dga</t>
   </si>
   <si>
@@ -2330,6 +2327,9 @@
   </si>
   <si>
     <t>cambiar silica cuba</t>
+  </si>
+  <si>
+    <t>muestra de aceite</t>
   </si>
 </sst>
 </file>
@@ -2692,8 +2692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4652E69-929B-714C-BC33-EF63CEFF457E}">
   <dimension ref="A1:C115"/>
   <sheetViews>
-    <sheetView zoomScale="108" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2748,7 +2748,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>752</v>
+        <v>762</v>
       </c>
       <c r="C7" t="s">
         <v>743</v>
@@ -2807,7 +2807,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="C16" t="s">
         <v>744</v>
@@ -2950,7 +2950,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="C39" t="s">
         <v>745</v>
@@ -3464,7 +3464,7 @@
         <v>115</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="C5" t="s">
         <v>128</v>
@@ -3499,7 +3499,7 @@
         <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="C10" t="s">
         <v>129</v>
@@ -3648,7 +3648,7 @@
         <v>134</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C6" t="s">
         <v>746</v>
@@ -3797,7 +3797,7 @@
         <v>150</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="C6" t="s">
         <v>359</v>
@@ -3826,7 +3826,7 @@
         <v>154</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C10" t="s">
         <v>747</v>
@@ -3837,7 +3837,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C11" t="s">
         <v>128</v>
@@ -5402,7 +5402,7 @@
         <v>154</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C4" t="s">
         <v>747</v>
@@ -5665,7 +5665,7 @@
         <v>150</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="C7" t="s">
         <v>748</v>
@@ -6275,7 +6275,7 @@
         <v>508</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="C107" t="s">
         <v>678</v>
@@ -7412,7 +7412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB803BC0-B6CC-AE49-9A0F-3FBDF262121B}">
   <dimension ref="A1:C92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="125" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -7457,7 +7457,7 @@
         <v>425</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="C5" t="s">
         <v>677</v>
@@ -7600,7 +7600,7 @@
         <v>700</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C28" t="s">
         <v>741</v>
@@ -7617,7 +7617,7 @@
         <v>491</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C30" t="s">
         <v>677</v>
@@ -7760,7 +7760,7 @@
         <v>269</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C53" t="s">
         <v>742</v>

</xml_diff>